<commit_message>
add ticket category + price in dataset
</commit_message>
<xml_diff>
--- a/raw_dataset.xlsx
+++ b/raw_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telkom University\Semester 6\Penulisan Proposal\penting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ED4961-5844-4B54-8262-FAA881A36AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1E5ED2-DA0F-4670-B10B-6CB116C1572A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FA70D09C-F239-4C1A-B6E5-6684D0D82B42}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{FA70D09C-F239-4C1A-B6E5-6684D0D82B42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="407">
   <si>
     <t>Art: 1 New Museum</t>
   </si>
@@ -1081,6 +1081,180 @@
   </si>
   <si>
     <t>ppiptek</t>
+  </si>
+  <si>
+    <t>125000, 100000, 75000, 0</t>
+  </si>
+  <si>
+    <t>Umum</t>
+  </si>
+  <si>
+    <t>Dewasa, Anak - Anak</t>
+  </si>
+  <si>
+    <t>20000, 10000</t>
+  </si>
+  <si>
+    <t>7500, 3500</t>
+  </si>
+  <si>
+    <t>entry_ticket_category</t>
+  </si>
+  <si>
+    <t>entry_ticket_price</t>
+  </si>
+  <si>
+    <t>Pelataran Puncak</t>
+  </si>
+  <si>
+    <t>Dewasa, Anak - Anak, Pelajar</t>
+  </si>
+  <si>
+    <t>4000, 2500, 2500</t>
+  </si>
+  <si>
+    <t>Rombongan</t>
+  </si>
+  <si>
+    <t>other_ticket_category</t>
+  </si>
+  <si>
+    <t>other_ticket_name</t>
+  </si>
+  <si>
+    <t>Rombongan (Min. 40 Orang)</t>
+  </si>
+  <si>
+    <t>3000, 2000</t>
+  </si>
+  <si>
+    <t>2000, 1000</t>
+  </si>
+  <si>
+    <t>Gratis</t>
+  </si>
+  <si>
+    <t>other_ticket_price</t>
+  </si>
+  <si>
+    <t>Dewasa, Anak - Anak, Wisatawan Mancanegara</t>
+  </si>
+  <si>
+    <t>1000, 500, 10000</t>
+  </si>
+  <si>
+    <t>Dewasa, Pelajar</t>
+  </si>
+  <si>
+    <t>30000, 15000</t>
+  </si>
+  <si>
+    <t>Rombongan, Reservasi</t>
+  </si>
+  <si>
+    <t>25000, 15000</t>
+  </si>
+  <si>
+    <t>5000, 3000, 2000</t>
+  </si>
+  <si>
+    <t>Dewasa, Mahasiswa, Anak - Anak</t>
+  </si>
+  <si>
+    <t>3750, 2250, 1500</t>
+  </si>
+  <si>
+    <t>Dewasa, Mahasiswa, Pelajar</t>
+  </si>
+  <si>
+    <t>2000, 1000, 10000</t>
+  </si>
+  <si>
+    <t>4000, 2500</t>
+  </si>
+  <si>
+    <t>Dewasa, Pelajar, Anak - Anak, Lansia &gt; 65 Tahun</t>
+  </si>
+  <si>
+    <t>100000, 90000, 80000, 90000</t>
+  </si>
+  <si>
+    <t>Dewasa, Anak - Anak, Nasabah, Wisatawan Mancanegara</t>
+  </si>
+  <si>
+    <t>5000, 2000, 2000, 10000</t>
+  </si>
+  <si>
+    <t>5000, 2000, 10000</t>
+  </si>
+  <si>
+    <t>Rombongan (min. 10 Orang)</t>
+  </si>
+  <si>
+    <t>Dewasa, Anak - Anak (TK - SMP)</t>
+  </si>
+  <si>
+    <t>Dewasa, Anak - Anak (TK - SMP), Wisatawan Mancanegara</t>
+  </si>
+  <si>
+    <t>Rombongan (min. 20 Orang)</t>
+  </si>
+  <si>
+    <t>dapat Potongan 10%</t>
+  </si>
+  <si>
+    <t>Dewasa, Umum, Pelajar, Mahasiswa</t>
+  </si>
+  <si>
+    <t>5000, 5000, 3000, 3000</t>
+  </si>
+  <si>
+    <t>4000, 4000, 2000, 2000</t>
+  </si>
+  <si>
+    <t>Anak - Anak (TK dan SD), Dewasa</t>
+  </si>
+  <si>
+    <t>3000, 5000</t>
+  </si>
+  <si>
+    <t>Dewasa, Mahasiswa, HUT TNI 5 Oktober</t>
+  </si>
+  <si>
+    <t>4000, 2500, 0</t>
+  </si>
+  <si>
+    <t>Dewasa, Umum, Mahasiswa, Pelajar, Anak - Anak</t>
+  </si>
+  <si>
+    <t>5000, 5000, 3000, 2000, 2000</t>
+  </si>
+  <si>
+    <t>3750, 3750, 2250, 1500, 1500</t>
+  </si>
+  <si>
+    <t>Masuk, Pesawat, Kereta</t>
+  </si>
+  <si>
+    <t>5000, 3000, 5000</t>
+  </si>
+  <si>
+    <t>Dewasa, Mahasiswa, Pelajar, Anak - Anak</t>
+  </si>
+  <si>
+    <t>5000, 3000, 2000, 2000</t>
+  </si>
+  <si>
+    <t>Wisatawan Mancanegara, Umum, Pelajar, Anak - Anak &lt; 12 Tahun</t>
+  </si>
+  <si>
+    <t>Anak - Anak, Pelajar, Mahasiswa, Dewasa</t>
+  </si>
+  <si>
+    <t>2000, 2000, 3000, 5000</t>
+  </si>
+  <si>
+    <t>1500, 1500, 2250, 3750</t>
   </si>
 </sst>
 </file>
@@ -1125,13 +1299,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1447,26 +1623,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F55E5B-BB77-4DB5-B8B9-74475CF703C0}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="J29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="59.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="117.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="57.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="5" width="67.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="105.5703125" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
     <col min="8" max="8" width="26.7109375" customWidth="1"/>
     <col min="9" max="9" width="20.85546875" customWidth="1"/>
+    <col min="10" max="10" width="59.5703125" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" customWidth="1"/>
+    <col min="12" max="12" width="53.7109375" customWidth="1"/>
+    <col min="13" max="13" width="25.85546875" customWidth="1"/>
+    <col min="14" max="14" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>61</v>
       </c>
@@ -1494,8 +1675,23 @@
       <c r="I1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>354</v>
+      </c>
+      <c r="K1" t="s">
+        <v>355</v>
+      </c>
+      <c r="L1" t="s">
+        <v>360</v>
+      </c>
+      <c r="M1" t="s">
+        <v>361</v>
+      </c>
+      <c r="N1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1521,8 +1717,14 @@
       <c r="I2" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1550,8 +1752,14 @@
       <c r="I3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>350</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1573,8 +1781,14 @@
       <c r="H4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1602,8 +1816,14 @@
       <c r="I5" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>350</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1619,8 +1839,23 @@
       <c r="E6" s="5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>351</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="L6" t="s">
+        <v>351</v>
+      </c>
+      <c r="M6" t="s">
+        <v>356</v>
+      </c>
+      <c r="N6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1639,8 +1874,23 @@
       <c r="F7" s="4" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>357</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="L7" t="s">
+        <v>351</v>
+      </c>
+      <c r="M7" t="s">
+        <v>362</v>
+      </c>
+      <c r="N7" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1665,8 +1915,14 @@
       <c r="H8" s="3" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>350</v>
+      </c>
+      <c r="K8" s="6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1682,8 +1938,14 @@
       <c r="F9" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>350</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1705,8 +1967,14 @@
       <c r="H10" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>350</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1725,8 +1993,14 @@
       <c r="F11" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>350</v>
+      </c>
+      <c r="K11" s="6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1745,8 +2019,14 @@
       <c r="H12" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>351</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1774,8 +2054,14 @@
       <c r="I13" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>350</v>
+      </c>
+      <c r="K13" s="6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1788,8 +2074,14 @@
       <c r="D14" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>350</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1817,8 +2109,23 @@
       <c r="I15" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>351</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1837,8 +2144,14 @@
       <c r="F16" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>350</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1851,8 +2164,14 @@
       <c r="D17" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>350</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1880,8 +2199,14 @@
       <c r="I18" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>369</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1909,8 +2234,14 @@
       <c r="I19" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>350</v>
+      </c>
+      <c r="K19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -1929,8 +2260,14 @@
       <c r="I20" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>371</v>
+      </c>
+      <c r="K20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1958,8 +2295,14 @@
       <c r="I21" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>350</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1978,8 +2321,14 @@
       <c r="F22" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>350</v>
+      </c>
+      <c r="K22" s="6">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -2007,8 +2356,14 @@
       <c r="I23" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>351</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -2030,8 +2385,14 @@
       <c r="I24" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>350</v>
+      </c>
+      <c r="K24" s="6">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -2053,8 +2414,14 @@
       <c r="H25" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>350</v>
+      </c>
+      <c r="K25" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -2079,8 +2446,14 @@
       <c r="I26" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>350</v>
+      </c>
+      <c r="K26" s="6">
+        <v>185000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -2099,8 +2472,14 @@
       <c r="F27" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>350</v>
+      </c>
+      <c r="K27" s="6">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
@@ -2113,8 +2492,14 @@
       <c r="D28" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>350</v>
+      </c>
+      <c r="K28" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
@@ -2136,8 +2521,23 @@
       <c r="H29" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>374</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
@@ -2156,8 +2556,14 @@
       <c r="F30" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>350</v>
+      </c>
+      <c r="K30" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
@@ -2183,8 +2589,14 @@
       <c r="I31" s="4" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
@@ -2209,8 +2621,14 @@
       <c r="I32" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
@@ -2229,8 +2647,14 @@
       <c r="F33" s="4" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>32</v>
       </c>
@@ -2258,8 +2682,14 @@
       <c r="I34" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K34" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
@@ -2281,8 +2711,14 @@
       <c r="H35" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K35" s="6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
@@ -2307,8 +2743,14 @@
       <c r="I36" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K36" s="6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
@@ -2336,8 +2778,14 @@
       <c r="I37" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -2365,8 +2813,14 @@
       <c r="I38" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
@@ -2385,8 +2839,23 @@
       <c r="H39" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
@@ -2414,8 +2883,14 @@
       <c r="I40" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
@@ -2443,8 +2918,23 @@
       <c r="I41" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="N41" s="7" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
@@ -2472,8 +2962,14 @@
       <c r="I42" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K42" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>41</v>
       </c>
@@ -2498,8 +2994,14 @@
       <c r="I43" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K43" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>42</v>
       </c>
@@ -2524,8 +3026,23 @@
       <c r="I44" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="N44" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>43</v>
       </c>
@@ -2550,8 +3067,14 @@
       <c r="H45" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K45" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>44</v>
       </c>
@@ -2567,8 +3090,20 @@
       <c r="F46" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K46" s="6">
+        <v>5000</v>
+      </c>
+      <c r="L46" t="s">
+        <v>388</v>
+      </c>
+      <c r="M46" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>45</v>
       </c>
@@ -2590,8 +3125,23 @@
       <c r="I47" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="K47" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="N47" s="7" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>46</v>
       </c>
@@ -2610,8 +3160,14 @@
       <c r="F48" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>47</v>
       </c>
@@ -2627,8 +3183,14 @@
       <c r="E49" s="3" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K49" s="6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>48</v>
       </c>
@@ -2650,8 +3212,14 @@
       <c r="G50" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K50" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>49</v>
       </c>
@@ -2664,8 +3232,14 @@
       <c r="D51" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K51" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>50</v>
       </c>
@@ -2687,8 +3261,14 @@
       <c r="I52" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="K52" s="7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>51</v>
       </c>
@@ -2701,8 +3281,14 @@
       <c r="D53" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>52</v>
       </c>
@@ -2727,8 +3313,23 @@
       <c r="I54" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="K54" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="L54" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="M54" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="N54" s="7" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>53</v>
       </c>
@@ -2747,8 +3348,14 @@
       <c r="F55" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K55" s="6">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>54</v>
       </c>
@@ -2776,8 +3383,23 @@
       <c r="I56" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="L56" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="M56" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="N56" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>55</v>
       </c>
@@ -2799,8 +3421,23 @@
       <c r="I57" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="L57" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="M57" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="N57" s="7" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>56</v>
       </c>
@@ -2819,8 +3456,14 @@
       <c r="F58" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K58" s="6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>57</v>
       </c>
@@ -2845,8 +3488,14 @@
       <c r="I59" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K59" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>58</v>
       </c>
@@ -2868,8 +3517,14 @@
       <c r="H60" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="K60" s="7" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>59</v>
       </c>
@@ -2888,8 +3543,14 @@
       <c r="H61" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="K61" s="7" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>60</v>
       </c>
@@ -2916,6 +3577,12 @@
       </c>
       <c r="I62" t="s">
         <v>348</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="K62" s="6">
+        <v>16500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add transport, longitude, latitude field
</commit_message>
<xml_diff>
--- a/raw_dataset.xlsx
+++ b/raw_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Telkom University\Semester 6\Penulisan Proposal\penting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1E5ED2-DA0F-4670-B10B-6CB116C1572A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7F448C-6A02-46D9-A524-6A56BFEE48A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{FA70D09C-F239-4C1A-B6E5-6684D0D82B42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="655" xr2:uid="{FA70D09C-F239-4C1A-B6E5-6684D0D82B42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="509">
   <si>
     <t>Art: 1 New Museum</t>
   </si>
@@ -282,9 +282,6 @@
     <t>Gedung Nusantara Lantai 2 Komp. MPR, DPR, DPD RI Jl. Jenderal Gatot Subroto, Senayan, Jakarta Pusat</t>
   </si>
   <si>
-    <t>Jl. Salemba Raya No. 6 Kenari, Senen, Jakarta Pusat</t>
-  </si>
-  <si>
     <t>Jl. Cilandak Tengah No.71, RT.2/RW.13, Cilandak Barat, Cilandak, Jakarta Selatan</t>
   </si>
   <si>
@@ -1255,6 +1252,315 @@
   </si>
   <si>
     <t>1500, 1500, 2250, 3750</t>
+  </si>
+  <si>
+    <t>distance_to_museum</t>
+  </si>
+  <si>
+    <t>place_to_museum</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>26.9, 0.75, 3.2, 4.4, 5.7</t>
+  </si>
+  <si>
+    <t>45, 10, 20.4, 22.6, 13, 4.3</t>
+  </si>
+  <si>
+    <t>29, 14, 1, 3, 3</t>
+  </si>
+  <si>
+    <t>Bandara Halim Perdanakusuma, Stasiun Rajawali, Stasiun Sawah Besar, Stasiun Kemayoran, Terminal Senen</t>
+  </si>
+  <si>
+    <t>28.6, 20.4, 22.7, 13,3</t>
+  </si>
+  <si>
+    <t>0.85, 3, 4, 4, 16, 30</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Stasiun Gambir, Stasiun Pasar Senen, Terminal Pasar Senen</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Terminal Kampung Rambutan, Terminal Rawamangun</t>
+  </si>
+  <si>
+    <t>11, 53, 23, 23, 23, 23</t>
+  </si>
+  <si>
+    <t>39.8, 9.2, 3.9, 6.1, 18.3, 5.6</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Stasiun Pasar Senen, Stasiun Gambir, Terminal Rawamangun, Terminal Kampung Rambutan</t>
+  </si>
+  <si>
+    <t>Stasiun Gambir, Stasiun Pasar Senen, Terminal Tanah Abang, Terminal Manggarai, Bandara Halim Perdanakusuma, Bandara Soekarno - Hatta</t>
+  </si>
+  <si>
+    <t>Bandara Halim Perdanakusuma, Bandara Soekarno - Hatta, Stasiun Gambir, Stasiun Pasar Senen, Terminal Senen, Terminal Tanah Abang</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Stasiun Pasar Senen, Stasiun Gambir, Terminal Kampung Rambutan, Terminal Rawamangun</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Stasiun Gambir, Stasiun Pasar Senen, Terminal Rawamangun, Terminal Kampung Rambutan</t>
+  </si>
+  <si>
+    <t>33.3, 18.6, 19.9, 22.3, 29.6, 13.6</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Stasiun Gambir, Stasiun Pasar Senen, Terminal Kampung Rambutan, Terminal Rawamangun</t>
+  </si>
+  <si>
+    <t>19.5, 39, 11, 14.1, 29.4, 22.3</t>
+  </si>
+  <si>
+    <t>44.6, 10.6, 22.6, 20.4, 3.3, 16.3</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Terminal Rawamangun, Terminal Kampung Rambutan</t>
+  </si>
+  <si>
+    <t>20.8, 25.8, 24.2, 31.7</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Terminal Rawamangun</t>
+  </si>
+  <si>
+    <t>21.8, 31, 20</t>
+  </si>
+  <si>
+    <t>26.2, 16.8, 3.6, 5.9, 13.2, 25.8</t>
+  </si>
+  <si>
+    <t>34.4, 20.9, 19, 18, 10.8, 21.5</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Stasiun Jakarta Utara, Terminal Pulo Gadung</t>
+  </si>
+  <si>
+    <t>32, 12, 10.9</t>
+  </si>
+  <si>
+    <t>22.2, 27.2, 19.5, 31.8</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Stasiun Sudirman, Stasiun Tebet, Terminal Manggarai</t>
+  </si>
+  <si>
+    <t>29.9, 2.8, 3.9, 6.4</t>
+  </si>
+  <si>
+    <t>28, 18, 0.5, 3, 3</t>
+  </si>
+  <si>
+    <t>Stasiun Pasar Minggu, Stasiun Cawang, Terminal Pasar Minggu</t>
+  </si>
+  <si>
+    <t>6, 6.9, 4.8</t>
+  </si>
+  <si>
+    <t>18, 11, 6.6, 5.1, 14, 10</t>
+  </si>
+  <si>
+    <t>11.9, 23.9, 21.7, 5.6, 17.6</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Stasiun Gondangdia, Stasiun Gambir</t>
+  </si>
+  <si>
+    <t>40, 3.8, 5</t>
+  </si>
+  <si>
+    <t>Jl. Salemba Raya No. 6, Kenari, Senen, Jakarta Pusat</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Stasiun Gambir, Terminal Kampung Rambutan, Terminal Rawamangun</t>
+  </si>
+  <si>
+    <t>45.9, 11.8, 23.8, 5.6, 17.6</t>
+  </si>
+  <si>
+    <t>48, 12.3, 15.1, 6.8</t>
+  </si>
+  <si>
+    <t>Stasiun Tanjung Barat, Terminal Pasar Minggu</t>
+  </si>
+  <si>
+    <t>6.4, 8.8</t>
+  </si>
+  <si>
+    <t>45.9, 10.2, 22.2, 20, 5.6, 15</t>
+  </si>
+  <si>
+    <t>2.6, 3.8, 4</t>
+  </si>
+  <si>
+    <t>Stasiun Sudirman, Stasiun Manggarai, Terminal Manggarai</t>
+  </si>
+  <si>
+    <t>Bandara Halim Perdanakusuma, Bandara Soekarno - Hatta, Stasiun Gambir, Stasiun Senen, Terminal Senen, Terminal Tanah Abang, Terminal Manggarai</t>
+  </si>
+  <si>
+    <t>13, 30, 3, 3, 3, 4, 5</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Stasiun Juanda</t>
+  </si>
+  <si>
+    <t>28.2, 1.2</t>
+  </si>
+  <si>
+    <t>Bandara Halim Perdanakusuma, Stasiun Pasar Senen, Terminal Senen</t>
+  </si>
+  <si>
+    <t>15, 1, 1</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Stasiun Palmerah, Stasiun Karet, Stasiun Gambir</t>
+  </si>
+  <si>
+    <t>26.9, 3.1, 3.8, 8.2</t>
+  </si>
+  <si>
+    <t>46.4, 12.3, 24.3, 22.1, 6, 18.1</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Stasiun Gambir, Terminal Rawamangun</t>
+  </si>
+  <si>
+    <t>30, 14, 3, 10</t>
+  </si>
+  <si>
+    <t>Bandara Halim Perdanakusuma, Stasiun Tanah Abang, Terminal Blok M</t>
+  </si>
+  <si>
+    <t>22, 18, 9</t>
+  </si>
+  <si>
+    <t>46, 12, 22.6, 23.6, 15, 5.7</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Stasiun Palmerah, Halte Busway Kebon Jeruk</t>
+  </si>
+  <si>
+    <t>27.2, 8.3, 0.4</t>
+  </si>
+  <si>
+    <t>21.3, 23.9, 5.7, 7.6, 21.6, 33.9</t>
+  </si>
+  <si>
+    <t>Stasiun Sentiong, Stasiun Cikini, Terminal Pasar Senen</t>
+  </si>
+  <si>
+    <t>2.3, 3, 4</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Stasiun Juanda, Stasiun Gambir</t>
+  </si>
+  <si>
+    <t>29.6, 3.9, 3.5</t>
+  </si>
+  <si>
+    <t>45.8, 10.2, 24.4, 22.1, 4, 16</t>
+  </si>
+  <si>
+    <t>Bandara Udara Soekarno - Hatta, Bandara Halim Perdanakusuma, Terminal Rawamangun, Terminal Kampung Rambutan</t>
+  </si>
+  <si>
+    <t>45.3, 11.2, 14, 4.9</t>
+  </si>
+  <si>
+    <t>44.6, 10.6, 13.4, 4.3</t>
+  </si>
+  <si>
+    <t>30.8, 14, 5.3, 5.9, 20.3, 11.1</t>
+  </si>
+  <si>
+    <t>31.4, 13.8, 12.7, 12.6, 21.1, 17.6</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Stasiun Gambir, Stasiun Pasar Senen,Terminal Rawamangun, Terminal Kampung Rambutan</t>
+  </si>
+  <si>
+    <t>46, 12, 24, 21.8, 15, 5.7</t>
+  </si>
+  <si>
+    <t>Bandara Halim Perdanakusuma, Stasiun Tanah Abang, Terminal Grogol, Terminal Kampung Melayu</t>
+  </si>
+  <si>
+    <t>18, 3, 4, 10</t>
+  </si>
+  <si>
+    <t>Bandara Halim Perdanakusuma, Stasiun Tanjung Barat, Terminal Kampung Rambutan</t>
+  </si>
+  <si>
+    <t>10.5, 11, 3.2</t>
+  </si>
+  <si>
+    <t>46.4, 12.3, 22.2, 20, 6.1</t>
+  </si>
+  <si>
+    <t>Stasiun Juanda, Stasiun Gambir, Terminal Pasar Senen</t>
+  </si>
+  <si>
+    <t>0.85, 3.2, 2.7</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Stasiun Gambir, Stasiun Pasar Senen, Terminal Senen, Terminal Tanah Abang, Terminal Manggarai</t>
+  </si>
+  <si>
+    <t>33, 12, 5, 6, 6, 6, 2</t>
+  </si>
+  <si>
+    <t>13, 6, 5</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Stasiun Kota, Stasiun Pasar Senen, Stasiun Gambir, Terminal Senen</t>
+  </si>
+  <si>
+    <t>23, 26, 0.8, 7, 6.7, 7</t>
+  </si>
+  <si>
+    <t>21.6, 25, 8.8, 6.4, 30.7, 24.9</t>
+  </si>
+  <si>
+    <t>46, 12, 15, 6.1</t>
+  </si>
+  <si>
+    <t>31.9, 14.7, 1.9, 4.1, 19.7, 10.3</t>
+  </si>
+  <si>
+    <t>Bandara Soekarno - Hatta, Bandara Halim Perdanakusuma, Stasiun Gambir, Stasiun Pasar Senen, Terminal Kampung Rambutan</t>
+  </si>
+  <si>
+    <t>27.8, 18.6, 5.1, 7.5, 21.8</t>
+  </si>
+  <si>
+    <t>Bandara Halim Perdanakusuma, Stasiun Gambir, Stasiun Pasar Senen, Terminal Kampung Rambutan</t>
+  </si>
+  <si>
+    <t>11, 23, 21, 5</t>
+  </si>
+  <si>
+    <t>Stasiun Grogol, Terminal Kalideres, Pulo Gadung, Bandara Halim Perdanakusuma, Bandara Soekarno - Hatta</t>
+  </si>
+  <si>
+    <t>4.7, 13.9, 16.1, 18.2, 25.2</t>
+  </si>
+  <si>
+    <t>46, 12, 23.9, 21.7, 5.7, 17,7</t>
+  </si>
+  <si>
+    <t>21, 24, 6, 8, 27, 30</t>
+  </si>
+  <si>
+    <t>46.2, 11.9, 24.1, 24, 5.8, 16.4</t>
   </si>
 </sst>
 </file>
@@ -1623,10 +1929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F55E5B-BB77-4DB5-B8B9-74475CF703C0}">
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" topLeftCell="K40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R62" sqref="R62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,9 +1951,13 @@
     <col min="12" max="12" width="53.7109375" customWidth="1"/>
     <col min="13" max="13" width="25.85546875" customWidth="1"/>
     <col min="14" max="14" width="26" customWidth="1"/>
+    <col min="15" max="15" width="24.140625" customWidth="1"/>
+    <col min="16" max="16" width="29.42578125" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>61</v>
       </c>
@@ -1655,43 +1965,55 @@
         <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
         <v>113</v>
       </c>
-      <c r="F1" t="s">
-        <v>114</v>
-      </c>
       <c r="G1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I1" t="s">
         <v>221</v>
       </c>
-      <c r="H1" t="s">
-        <v>220</v>
-      </c>
-      <c r="I1" t="s">
-        <v>222</v>
-      </c>
       <c r="J1" t="s">
+        <v>353</v>
+      </c>
+      <c r="K1" t="s">
         <v>354</v>
       </c>
-      <c r="K1" t="s">
-        <v>355</v>
-      </c>
       <c r="L1" t="s">
+        <v>359</v>
+      </c>
+      <c r="M1" t="s">
         <v>360</v>
       </c>
-      <c r="M1" t="s">
-        <v>361</v>
-      </c>
       <c r="N1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+      <c r="O1" t="s">
+        <v>407</v>
+      </c>
+      <c r="P1" t="s">
+        <v>406</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>408</v>
+      </c>
+      <c r="R1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1699,32 +2021,44 @@
         <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+      <c r="O2" t="s">
+        <v>413</v>
+      </c>
+      <c r="P2" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q2">
+        <v>-6.1469501733805796</v>
+      </c>
+      <c r="R2">
+        <v>106.84028946174401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1732,34 +2066,46 @@
         <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K3" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>420</v>
+      </c>
+      <c r="P3" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q3">
+        <v>-6.3027984985778698</v>
+      </c>
+      <c r="R3">
+        <v>106.88786250715999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1767,28 +2113,40 @@
         <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="G4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K4" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>416</v>
+      </c>
+      <c r="P4" t="s">
+        <v>412</v>
+      </c>
+      <c r="Q4">
+        <v>-6.1658974997396498</v>
+      </c>
+      <c r="R4">
+        <v>106.833966529085</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1796,34 +2154,46 @@
         <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="F5" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="H5" t="s">
         <v>234</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>235</v>
       </c>
-      <c r="I5" t="s">
-        <v>236</v>
-      </c>
       <c r="J5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>417</v>
+      </c>
+      <c r="P5" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q5">
+        <v>-6.1785499519907798</v>
+      </c>
+      <c r="R5">
+        <v>106.83277191867199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1831,31 +2201,43 @@
         <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="J6" t="s">
+        <v>350</v>
+      </c>
+      <c r="K6" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="L6" t="s">
+        <v>350</v>
+      </c>
+      <c r="M6" t="s">
+        <v>355</v>
+      </c>
+      <c r="N6" t="s">
         <v>352</v>
       </c>
-      <c r="L6" t="s">
-        <v>351</v>
-      </c>
-      <c r="M6" t="s">
-        <v>356</v>
-      </c>
-      <c r="N6" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>421</v>
+      </c>
+      <c r="P6" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q6">
+        <v>-6.1753935482312503</v>
+      </c>
+      <c r="R6">
+        <v>106.827151981719</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1863,34 +2245,46 @@
         <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J7" t="s">
+        <v>356</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="K7" s="6" t="s">
-        <v>358</v>
-      </c>
       <c r="L7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M7" t="s">
+        <v>361</v>
+      </c>
+      <c r="N7" t="s">
         <v>362</v>
       </c>
-      <c r="N7" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>422</v>
+      </c>
+      <c r="P7" t="s">
+        <v>418</v>
+      </c>
+      <c r="Q7">
+        <v>-6.2903171193619603</v>
+      </c>
+      <c r="R7">
+        <v>106.90859647079201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1898,31 +2292,43 @@
         <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="F8" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>240</v>
-      </c>
       <c r="J8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K8" s="6">
         <v>5000</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>423</v>
+      </c>
+      <c r="P8" t="s">
+        <v>419</v>
+      </c>
+      <c r="Q8">
+        <v>-6.1963101616413798</v>
+      </c>
+      <c r="R8">
+        <v>106.849993043258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1930,22 +2336,34 @@
         <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K9" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>424</v>
+      </c>
+      <c r="P9" t="s">
+        <v>425</v>
+      </c>
+      <c r="Q9">
+        <v>-6.2910499408183904</v>
+      </c>
+      <c r="R9">
+        <v>106.771567493006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1953,28 +2371,40 @@
         <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>130</v>
-      </c>
       <c r="F10" t="s">
+        <v>241</v>
+      </c>
+      <c r="H10" t="s">
         <v>242</v>
       </c>
-      <c r="H10" t="s">
-        <v>243</v>
-      </c>
       <c r="J10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K10" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>426</v>
+      </c>
+      <c r="P10" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q10">
+        <v>-6.1252003690329397</v>
+      </c>
+      <c r="R10">
+        <v>106.793359599637</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1982,25 +2412,37 @@
         <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>132</v>
-      </c>
       <c r="F11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K11" s="6">
         <v>10000</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>426</v>
+      </c>
+      <c r="P11" t="s">
+        <v>428</v>
+      </c>
+      <c r="Q11">
+        <v>-6.3073173436541596</v>
+      </c>
+      <c r="R11">
+        <v>106.894176875479</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -2008,25 +2450,37 @@
         <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="H12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+      <c r="O12" t="s">
+        <v>429</v>
+      </c>
+      <c r="P12" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q12">
+        <v>-6.1275397928704596</v>
+      </c>
+      <c r="R12">
+        <v>106.809071555342</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -2034,34 +2488,46 @@
         <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="F13" t="s">
+        <v>244</v>
+      </c>
+      <c r="G13" t="s">
         <v>245</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>246</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>247</v>
       </c>
-      <c r="I13" t="s">
-        <v>248</v>
-      </c>
       <c r="J13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K13" s="6">
         <v>5000</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>431</v>
+      </c>
+      <c r="P13" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q13">
+        <v>-6.1371336262278096</v>
+      </c>
+      <c r="R13">
+        <v>106.81300122728901</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -2069,19 +2535,31 @@
         <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+      <c r="O14" t="s">
+        <v>424</v>
+      </c>
+      <c r="P14" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q14">
+        <v>-6.1671849290241996</v>
+      </c>
+      <c r="R14">
+        <v>106.820300697745</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -2089,43 +2567,55 @@
         <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>139</v>
-      </c>
       <c r="F15" t="s">
+        <v>248</v>
+      </c>
+      <c r="G15" t="s">
+        <v>251</v>
+      </c>
+      <c r="H15" t="s">
         <v>249</v>
       </c>
-      <c r="G15" t="s">
-        <v>252</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>250</v>
       </c>
-      <c r="I15" t="s">
-        <v>251</v>
-      </c>
       <c r="J15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L15" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="N15" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="Q15">
+        <v>-6.2897778311939403</v>
+      </c>
+      <c r="R15">
+        <v>106.79325736891001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -2133,45 +2623,69 @@
         <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K16" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>436</v>
+      </c>
+      <c r="Q16">
+        <v>-6.1416742665790203</v>
+      </c>
+      <c r="R16">
+        <v>106.901586885387</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K17" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q17">
+        <v>-6.1358232472997303</v>
+      </c>
+      <c r="R17">
+        <v>106.814334157414</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -2179,34 +2693,46 @@
         <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>143</v>
-      </c>
       <c r="F18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J18" t="s">
+        <v>368</v>
+      </c>
+      <c r="K18" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="K18" s="6" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="6" t="s">
+        <v>438</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q18">
+        <v>-6.2241048784007296</v>
+      </c>
+      <c r="R18">
+        <v>106.82389679689101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -2214,34 +2740,46 @@
         <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>145</v>
-      </c>
       <c r="F19" t="s">
+        <v>255</v>
+      </c>
+      <c r="G19" t="s">
         <v>256</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
+        <v>256</v>
+      </c>
+      <c r="I19" t="s">
         <v>257</v>
       </c>
-      <c r="H19" t="s">
-        <v>257</v>
-      </c>
-      <c r="I19" t="s">
-        <v>258</v>
-      </c>
       <c r="J19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K19" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q19">
+        <v>-6.1738474508070098</v>
+      </c>
+      <c r="R19">
+        <v>106.830425628578</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -2249,25 +2787,37 @@
         <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H20" t="s">
+        <v>258</v>
+      </c>
+      <c r="I20" t="s">
         <v>259</v>
       </c>
-      <c r="I20" t="s">
-        <v>260</v>
-      </c>
       <c r="J20" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K20" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="Q20">
+        <v>-6.2675150072628298</v>
+      </c>
+      <c r="R20">
+        <v>106.824082554965</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -2275,34 +2825,46 @@
         <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="F21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J21" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K21" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="Q21">
+        <v>-6.2104437331357296</v>
+      </c>
+      <c r="R21">
+        <v>106.799762674783</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -2310,60 +2872,84 @@
         <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="F22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K22" s="6">
         <v>25000</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q22">
+        <v>-6.3036601776024099</v>
+      </c>
+      <c r="R22">
+        <v>106.901011732748</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>82</v>
+        <v>447</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
+        <v>266</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F23" t="s">
+        <v>264</v>
+      </c>
+      <c r="G23" t="s">
         <v>267</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="F23" t="s">
-        <v>265</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>268</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>269</v>
       </c>
-      <c r="I23" t="s">
-        <v>270</v>
-      </c>
       <c r="J23" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q23">
+        <v>-6.1951565920131397</v>
+      </c>
+      <c r="R23">
+        <v>106.848372493646</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -2371,28 +2957,40 @@
         <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="H24" t="s">
+        <v>270</v>
+      </c>
+      <c r="I24" t="s">
         <v>271</v>
       </c>
-      <c r="I24" t="s">
-        <v>272</v>
-      </c>
       <c r="J24" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K24" s="6">
         <v>15000</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>449</v>
+      </c>
+      <c r="Q24">
+        <v>-6.3022461276546</v>
+      </c>
+      <c r="R24">
+        <v>106.90496512262099</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -2400,60 +2998,84 @@
         <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D25" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="F25" t="s">
+        <v>272</v>
+      </c>
+      <c r="H25" t="s">
         <v>273</v>
       </c>
-      <c r="H25" t="s">
-        <v>274</v>
-      </c>
       <c r="J25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K25" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="Q25">
+        <v>-6.3051878789188596</v>
+      </c>
+      <c r="R25">
+        <v>106.903966692444</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D26" t="s">
+        <v>274</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F26" t="s">
         <v>275</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="H26" t="s">
         <v>276</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>277</v>
       </c>
-      <c r="I26" t="s">
-        <v>278</v>
-      </c>
       <c r="J26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K26" s="6">
         <v>185000</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q26">
+        <v>-6.2889395055810802</v>
+      </c>
+      <c r="R26">
+        <v>106.801979083568</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -2461,174 +3083,246 @@
         <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="F27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J27" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K27" s="6">
         <v>15000</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="Q27">
+        <v>-6.3010491630791901</v>
+      </c>
+      <c r="R27">
+        <v>106.891443741804</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J28" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K28" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="P28" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q28">
+        <v>-6.1929602057138204</v>
+      </c>
+      <c r="R28">
+        <v>106.83266425206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D29" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="G29" t="s">
+        <v>279</v>
+      </c>
+      <c r="H29" t="s">
         <v>280</v>
       </c>
-      <c r="H29" t="s">
-        <v>281</v>
-      </c>
       <c r="J29" t="s">
+        <v>373</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="N29" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="K29" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="P29" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="Q29">
+        <v>-6.1861950350851203</v>
+      </c>
+      <c r="R29">
+        <v>106.836435641482</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D30" t="s">
+        <v>160</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>162</v>
-      </c>
       <c r="F30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J30" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K30" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="P30" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="Q30">
+        <v>-6.1688582907275498</v>
+      </c>
+      <c r="R30">
+        <v>106.83338436896901</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D31" t="s">
+        <v>162</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="F31" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="I31" s="4" t="s">
-        <v>286</v>
-      </c>
       <c r="J31" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q31">
+        <v>-6.1783519187355598</v>
+      </c>
+      <c r="R31">
+        <v>106.838093327206</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D32" t="s">
+        <v>164</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>166</v>
-      </c>
       <c r="G32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K32" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32" s="6" t="s">
+        <v>462</v>
+      </c>
+      <c r="P32" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="Q32">
+        <v>-6.2072157162471804</v>
+      </c>
+      <c r="R32">
+        <v>106.79886800833199</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
@@ -2636,89 +3330,125 @@
         <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D33" t="s">
+        <v>166</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="F33" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="P33" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="Q33">
+        <v>-6.3059455575344003</v>
+      </c>
+      <c r="R33">
+        <v>106.896853990311</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D34" t="s">
+        <v>168</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>170</v>
-      </c>
       <c r="F34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G34" t="s">
+        <v>288</v>
+      </c>
+      <c r="H34" t="s">
         <v>289</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>290</v>
       </c>
-      <c r="I34" t="s">
-        <v>291</v>
-      </c>
       <c r="J34" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K34" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="P34" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q34">
+        <v>-6.1741822330220701</v>
+      </c>
+      <c r="R34">
+        <v>106.837983599832</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s">
+        <v>171</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="G35" t="s">
+        <v>291</v>
+      </c>
+      <c r="H35" t="s">
         <v>292</v>
       </c>
-      <c r="H35" t="s">
-        <v>293</v>
-      </c>
       <c r="J35" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K35" s="6">
         <v>10000</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="P35" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="Q35">
+        <v>-6.3080287250402698</v>
+      </c>
+      <c r="R35">
+        <v>106.790547867261</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
@@ -2726,171 +3456,231 @@
         <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D36" t="s">
+        <v>173</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>175</v>
-      </c>
       <c r="F36" t="s">
+        <v>293</v>
+      </c>
+      <c r="H36" t="s">
+        <v>295</v>
+      </c>
+      <c r="I36" t="s">
         <v>294</v>
       </c>
-      <c r="H36" t="s">
-        <v>296</v>
-      </c>
-      <c r="I36" t="s">
-        <v>295</v>
-      </c>
       <c r="J36" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K36" s="6">
         <v>10000</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="P36" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q36">
+        <v>-6.30337267965868</v>
+      </c>
+      <c r="R36">
+        <v>106.904984756408</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D37" t="s">
+        <v>175</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="F37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H37" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J37" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="K37" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="K37" s="7" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="P37" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="Q37">
+        <v>-6.1909014467239603</v>
+      </c>
+      <c r="R37">
+        <v>106.76761947882601</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D38" t="s">
+        <v>177</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>179</v>
-      </c>
       <c r="F38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H38" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I38" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J38" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="K38" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="K38" s="7" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38" s="6" t="s">
+        <v>424</v>
+      </c>
+      <c r="P38" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="Q38">
+        <v>-6.1384499467172002</v>
+      </c>
+      <c r="R38">
+        <v>106.81330481482399</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D39" t="s">
+        <v>301</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H39" t="s">
         <v>302</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="H39" t="s">
-        <v>303</v>
-      </c>
       <c r="J39" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="K39" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="K39" s="6" t="s">
+      <c r="L39" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="N39" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="L39" s="6" t="s">
-        <v>404</v>
-      </c>
-      <c r="M39" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="N39" s="6" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="P39" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q39">
+        <v>-6.1935518832636198</v>
+      </c>
+      <c r="R39">
+        <v>106.84536153426799</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D40" t="s">
+        <v>180</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="F40" t="s">
+        <v>303</v>
+      </c>
+      <c r="G40" t="s">
+        <v>283</v>
+      </c>
+      <c r="H40" t="s">
         <v>304</v>
       </c>
-      <c r="G40" t="s">
-        <v>284</v>
-      </c>
-      <c r="H40" t="s">
-        <v>305</v>
-      </c>
       <c r="I40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K40" s="7" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+      <c r="O40" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="P40" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="Q40">
+        <v>-6.1764018346551497</v>
+      </c>
+      <c r="R40">
+        <v>106.82158989228</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
@@ -2898,43 +3688,55 @@
         <v>72</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D41" t="s">
+        <v>182</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="F41" t="s">
+        <v>305</v>
+      </c>
+      <c r="G41" t="s">
         <v>306</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>307</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>308</v>
       </c>
-      <c r="I41" t="s">
-        <v>309</v>
-      </c>
       <c r="J41" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="K41" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="K41" s="7" t="s">
+      <c r="L41" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="N41" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="L41" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="M41" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="N41" s="7" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="P41" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="Q41">
+        <v>-6.3042946731385001</v>
+      </c>
+      <c r="R41">
+        <v>106.889043716397</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
@@ -2942,34 +3744,46 @@
         <v>72</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D42" t="s">
+        <v>184</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>186</v>
-      </c>
       <c r="F42" t="s">
+        <v>309</v>
+      </c>
+      <c r="G42" t="s">
         <v>310</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>311</v>
       </c>
-      <c r="H42" t="s">
-        <v>312</v>
-      </c>
       <c r="I42" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K42" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="P42" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q42">
+        <v>-6.2994160635496099</v>
+      </c>
+      <c r="R42">
+        <v>106.898754728193</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>41</v>
       </c>
@@ -2977,104 +3791,140 @@
         <v>72</v>
       </c>
       <c r="C43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D43" t="s">
+        <v>186</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>188</v>
-      </c>
       <c r="F43" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I43" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K43" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="P43" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="Q43">
+        <v>-6.2991890555790198</v>
+      </c>
+      <c r="R43">
+        <v>106.893533180448</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D44" t="s">
+        <v>188</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="G44" t="s">
+        <v>318</v>
+      </c>
+      <c r="H44" t="s">
+        <v>318</v>
+      </c>
+      <c r="I44" t="s">
         <v>319</v>
       </c>
-      <c r="H44" t="s">
-        <v>319</v>
-      </c>
-      <c r="I44" t="s">
-        <v>320</v>
-      </c>
       <c r="J44" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="L44" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="K44" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="L44" s="7" t="s">
+      <c r="M44" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="M44" s="7" t="s">
-        <v>387</v>
-      </c>
       <c r="N44" s="7" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+      <c r="O44" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="P44" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q44">
+        <v>-6.2003749584424801</v>
+      </c>
+      <c r="R44">
+        <v>106.831007610052</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D45" t="s">
+        <v>190</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="F45" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G45" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H45" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K45" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="P45" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q45">
+        <v>-6.2393418780698999</v>
+      </c>
+      <c r="R45">
+        <v>106.802767930427</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>44</v>
       </c>
@@ -3082,28 +3932,40 @@
         <v>72</v>
       </c>
       <c r="C46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F46" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K46" s="6">
         <v>5000</v>
       </c>
       <c r="L46" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M46" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+      <c r="O46" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="P46" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="Q46">
+        <v>-6.3041845677159598</v>
+      </c>
+      <c r="R46">
+        <v>106.901771712265</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>45</v>
       </c>
@@ -3111,37 +3973,49 @@
         <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D47" t="s">
+        <v>193</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="E47" s="5" t="s">
-        <v>195</v>
-      </c>
       <c r="H47" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I47" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K47" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L47" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="M47" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N47" s="7" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+      <c r="O47" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="P47" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q47">
+        <v>-6.1722248114127902</v>
+      </c>
+      <c r="R47">
+        <v>106.818969026294</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>46</v>
       </c>
@@ -3149,25 +4023,37 @@
         <v>72</v>
       </c>
       <c r="C48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D48" t="s">
+        <v>195</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>197</v>
-      </c>
       <c r="F48" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J48" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="K48" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="K48" s="6" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="P48" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q48">
+        <v>-6.3003476889347896</v>
+      </c>
+      <c r="R48">
+        <v>106.886440970062</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>47</v>
       </c>
@@ -3175,161 +4061,233 @@
         <v>72</v>
       </c>
       <c r="C49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D49" t="s">
+        <v>197</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="J49" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K49" s="6">
         <v>10000</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="P49" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q49">
+        <v>-6.3052141027248503</v>
+      </c>
+      <c r="R49">
+        <v>106.89589033057899</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D50" t="s">
+        <v>199</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="F50" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G50" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K50" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="P50" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="Q50">
+        <v>-6.1669512894793002</v>
+      </c>
+      <c r="R50">
+        <v>106.825027430422</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D51" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K51" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="P51" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="Q51">
+        <v>-6.2046296428058598</v>
+      </c>
+      <c r="R51">
+        <v>106.836532665913</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C52" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D52" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F52" t="s">
+        <v>327</v>
+      </c>
+      <c r="H52" t="s">
         <v>328</v>
       </c>
-      <c r="H52" t="s">
-        <v>329</v>
-      </c>
       <c r="I52" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J52" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="K52" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="K52" s="7" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="P52" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="Q52">
+        <v>-6.2316989630693103</v>
+      </c>
+      <c r="R52">
+        <v>106.818542763548</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D53" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+      <c r="O53" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="P53" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="Q53">
+        <v>-6.13520026432625</v>
+      </c>
+      <c r="R53">
+        <v>106.813300112346</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C54" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D54" t="s">
+        <v>204</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>206</v>
-      </c>
       <c r="F54" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H54" t="s">
+        <v>329</v>
+      </c>
+      <c r="I54" t="s">
         <v>330</v>
       </c>
-      <c r="I54" t="s">
-        <v>331</v>
-      </c>
       <c r="J54" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="K54" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="K54" s="7" t="s">
+      <c r="L54" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="M54" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="N54" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="L54" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="M54" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="N54" s="7" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="P54" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q54">
+        <v>-6.1342182044104501</v>
+      </c>
+      <c r="R54">
+        <v>106.814692926147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>53</v>
       </c>
@@ -3337,107 +4295,143 @@
         <v>72</v>
       </c>
       <c r="C55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D55" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E55" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="F55" t="s">
         <v>333</v>
       </c>
-      <c r="F55" t="s">
-        <v>334</v>
-      </c>
       <c r="J55" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K55" s="6">
         <v>25000</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="P55" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="Q55">
+        <v>-6.3057427148999299</v>
+      </c>
+      <c r="R55">
+        <v>106.895463878659</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D56" t="s">
+        <v>334</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F56" t="s">
+        <v>336</v>
+      </c>
+      <c r="G56" t="s">
+        <v>315</v>
+      </c>
+      <c r="H56" t="s">
+        <v>315</v>
+      </c>
+      <c r="I56" t="s">
         <v>335</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="F56" t="s">
-        <v>337</v>
-      </c>
-      <c r="G56" t="s">
-        <v>316</v>
-      </c>
-      <c r="H56" t="s">
-        <v>316</v>
-      </c>
-      <c r="I56" t="s">
-        <v>336</v>
-      </c>
       <c r="J56" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K56" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L56" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="M56" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="N56" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="M56" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="N56" s="7" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="P56" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q56">
+        <v>-6.18379952050197</v>
+      </c>
+      <c r="R56">
+        <v>106.84310717115601</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D57" t="s">
+        <v>208</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="E57" s="5" t="s">
-        <v>210</v>
-      </c>
       <c r="H57" t="s">
+        <v>337</v>
+      </c>
+      <c r="I57" t="s">
         <v>338</v>
       </c>
-      <c r="I57" t="s">
-        <v>339</v>
-      </c>
       <c r="J57" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="K57" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="K57" s="7" t="s">
+      <c r="L57" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="M57" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="N57" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="L57" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="M57" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="N57" s="7" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="P57" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q57">
+        <v>-6.1879645292619596</v>
+      </c>
+      <c r="R57">
+        <v>106.809607366134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>56</v>
       </c>
@@ -3445,57 +4439,81 @@
         <v>72</v>
       </c>
       <c r="C58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D58" t="s">
+        <v>210</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>212</v>
-      </c>
       <c r="F58" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K58" s="6">
         <v>5000</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="P58" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q58">
+        <v>-6.3033150939248701</v>
+      </c>
+      <c r="R58">
+        <v>106.901455628741</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D59" t="s">
+        <v>212</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="E59" s="3" t="s">
-        <v>214</v>
-      </c>
       <c r="F59" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H59" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I59" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K59" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="P59" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="Q59">
+        <v>-6.1677099344560302</v>
+      </c>
+      <c r="R59">
+        <v>106.79050738195301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>58</v>
       </c>
@@ -3503,54 +4521,78 @@
         <v>72</v>
       </c>
       <c r="C60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D60" t="s">
+        <v>214</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="E60" s="5" t="s">
-        <v>216</v>
-      </c>
       <c r="F60" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H60" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J60" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="K60" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="K60" s="7" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="P60" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q60">
+        <v>-6.3049137581984702</v>
+      </c>
+      <c r="R60">
+        <v>106.898943393602</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C61" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D61" t="s">
+        <v>216</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="H61" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J61" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="K61" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="K61" s="7" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="P61" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q61">
+        <v>-6.13490616619183</v>
+      </c>
+      <c r="R61">
+        <v>106.812444552537</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>60</v>
       </c>
@@ -3558,35 +4600,50 @@
         <v>72</v>
       </c>
       <c r="C62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D62" t="s">
+        <v>346</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F62" t="s">
+        <v>345</v>
+      </c>
+      <c r="G62" t="s">
+        <v>344</v>
+      </c>
+      <c r="H62" t="s">
         <v>347</v>
       </c>
-      <c r="E62" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="F62" t="s">
-        <v>346</v>
-      </c>
-      <c r="G62" t="s">
-        <v>345</v>
-      </c>
-      <c r="H62" t="s">
-        <v>348</v>
-      </c>
       <c r="I62" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K62" s="6">
         <v>16500</v>
+      </c>
+      <c r="O62" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="P62" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q62">
+        <v>-6.3022187619334797</v>
+      </c>
+      <c r="R62">
+        <v>106.90357235395599</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="P31 P52" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>